<commit_message>
remove selection from main UI, change cursors, disable sort on row labels
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$15</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>Feature</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>Remove ability to drag-and-drop columns which contain row labels</t>
+  </si>
+  <si>
+    <t>N = length of rows array. First N elements of each row array do not have the draggable attribute. Sortable() attribute is on the TR, so will have to remove first N elements from sorting? (look up sortable({ items }) and add a selector to elements that CAN be sorted.</t>
   </si>
 </sst>
 </file>
@@ -683,10 +689,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +741,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -822,7 +829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -958,7 +965,31 @@
         <v>32</v>
       </c>
     </row>
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F15">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Not Started"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add error message for request timeout
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Feature</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Unsure what message CodeIgniter sends internally when request times out. Worst-case, front-end code can catch the HTTP 500 error and build an error object to show the user.</t>
   </si>
   <si>
-    <t>If the above mechanism works, do we need this functionality? The only downside to letting all requests complete on the back-end is that we are wasting DB queries. Otherwise, every server request is stateless so the requests don't affect each other.</t>
-  </si>
-  <si>
     <t>Make app UI discoverable for first-time users</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>Est Difficulty</t>
   </si>
   <si>
-    <t>Est. Time</t>
-  </si>
-  <si>
     <t>Implement query storage/retrieval and associated UI</t>
   </si>
   <si>
@@ -154,14 +148,17 @@
     <t>Remove ability to drag-and-drop columns which contain row labels</t>
   </si>
   <si>
-    <t>N = length of rows array. First N elements of each row array do not have the draggable attribute. Sortable() attribute is on the TR, so will have to remove first N elements from sorting? (look up sortable({ items }) and add a selector to elements that CAN be sorted.</t>
+    <t>N = length of rows array. First N elements of each row array do not have the sortable attribute.</t>
+  </si>
+  <si>
+    <t>If the associated front-end mechanism works, do we need this functionality? The only downside to letting all requests complete on the back-end is that we are wasting DB queries. Otherwise, every server request is stateless so the requests don't affect each other.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +169,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -198,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -223,6 +227,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,10 +697,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,13 +708,12 @@
     <col min="1" max="1" width="42.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="74.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -715,7 +721,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -723,45 +729,42 @@
       <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -771,225 +774,229 @@
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="E14" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="E15" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>39</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F15">
+  <autoFilter ref="A1:E16">
     <filterColumn colId="4">
       <filters>
         <filter val="Not Started"/>
       </filters>
     </filterColumn>
   </autoFilter>
+  <sortState ref="A2:F16">
+    <sortCondition ref="B2:B16"/>
+    <sortCondition ref="C2:C16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
expand model valdiations to include just rows/cols/vals
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>Feature</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Adjust jquery properties for draggable container.</t>
   </si>
   <si>
-    <t>Add logic to validation that does not reject this query configuration. This type of query will present a single row, COUNT(*).</t>
-  </si>
-  <si>
     <t>Add logic to validation that does not reject this query configuration. This type of query will present a single row, COUNT(*) pivoted against SELECT DISTINCT column values.</t>
   </si>
   <si>
@@ -152,6 +149,15 @@
   </si>
   <si>
     <t>If the associated front-end mechanism works, do we need this functionality? The only downside to letting all requests complete on the back-end is that we are wasting DB queries. Otherwise, every server request is stateless so the requests don't affect each other.</t>
+  </si>
+  <si>
+    <t>Fix 'column ambiguously defined' when aliasing long column values with aggregate fns</t>
+  </si>
+  <si>
+    <t>Look at deprecated column aliasing function. Take longest aggregate alias into account. Can these names be made more friendly? Or perhaps add metadata to the response so client can insert pretty column names?</t>
+  </si>
+  <si>
+    <t>Took this to mean 'only value(s) are selected'. Add logic to validation that does not reject this query configuration. This type of query will present a single row, COUNT(*).</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -230,6 +236,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,10 +718,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -730,77 +751,77 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -808,96 +829,96 @@
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
+      <c r="D6" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.25">
@@ -908,85 +929,102 @@
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="E15" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>31</v>
+      <c r="E17" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E16">
+  <autoFilter ref="A1:E17">
     <filterColumn colId="4">
       <filters>
         <filter val="Not Started"/>

</xml_diff>

<commit_message>
simple save/load last query
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -208,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -251,6 +251,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,7 +736,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,26 +766,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="1:5" s="13" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -779,41 +794,41 @@
         <v>5</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>30</v>
@@ -846,7 +861,7 @@
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -880,27 +895,27 @@
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4" t="s">
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>30</v>
       </c>
     </row>
@@ -914,27 +929,27 @@
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="4" t="s">
+    <row r="12" spans="1:5" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>30</v>
       </c>
     </row>
@@ -989,20 +1004,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="B16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="17" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1030,6 +1045,10 @@
         <filter val="Not Started"/>
       </filters>
     </filterColumn>
+    <sortState ref="A2:E17">
+      <sortCondition ref="B2:B17"/>
+      <sortCondition ref="C2:C17"/>
+    </sortState>
   </autoFilter>
   <sortState ref="A2:F16">
     <sortCondition ref="B2:B16"/>

</xml_diff>

<commit_message>
fix layout issues with long queries
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>Feature</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Ability to rename column row result values for first row /column (dropdowns are best)</t>
   </si>
   <si>
-    <t>HIGH/LOW</t>
-  </si>
-  <si>
     <t>Each query is assigned a unique ID when it is sent to server. Client maintains a buffer of pending queries. When user signals to halt current queries, results of queries in the buffer will be discarded when they return from the server. Queries made after the 'halt' command will be treated as normal.</t>
   </si>
   <si>
@@ -127,15 +124,9 @@
     <t>Est Difficulty</t>
   </si>
   <si>
-    <t>Implement query storage/retrieval and associated UI</t>
-  </si>
-  <si>
     <t>Query information is already being updated in lockstep with user actions. Trivial to store query objects (in localstorage to start with). On retrieval, fire off the stored query object and rearrange selection bucket DOM to match object. DOM arrangement will require rewriting some code in client-side View module.</t>
   </si>
   <si>
-    <t>Listing all values on a field (like Excel) will require a DB query, severely degrading user experience with the speeds we have been seeing.  On the flip side, allowing the user to combine multiple '___ OR ___' type criteria is low difficulty.</t>
-  </si>
-  <si>
     <t>Possibly. Best guess is to maintain an object describing transformations made to the 'base' pivot table returned from server, then applying transformations to a fresh copy of that query/table in a sensible order. There are a huge number of possible transformations that a user can make to the table, so this will be difficult to get 100% correct. Also we are concerned that this approach may not scale for future ways of displaying pivot table results.</t>
   </si>
   <si>
@@ -158,6 +149,24 @@
   </si>
   <si>
     <t>Took this to mean 'only value(s) are selected'. Add logic to validation that does not reject this query configuration. This type of query will present a single row, COUNT(*).</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Save/restore queries</t>
+  </si>
+  <si>
+    <t>Dropping a field into the filter bucket triggers a SELECT UNIQUE to get the field's values from the table. Values are available for manipulation from a right-click menu, replacing current filter interface.</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Bug: identical Value entries cause 'column ambiguously defined' (e.g. COUNTOF_ID and COUNTOF_ID in Values bucket)</t>
+  </si>
+  <si>
+    <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value.</t>
   </si>
 </sst>
 </file>
@@ -733,326 +742,395 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="17" t="s">
+      <c r="B10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="F13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="F16" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>30</v>
+      <c r="D18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E17">
-    <filterColumn colId="4">
+  <autoFilter ref="A1:F17">
+    <filterColumn colId="5">
       <filters>
+        <filter val="In progress"/>
         <filter val="Not Started"/>
       </filters>
     </filterColumn>
-    <sortState ref="A2:E17">
-      <sortCondition ref="B2:B17"/>
-      <sortCondition ref="C2:C17"/>
-    </sortState>
   </autoFilter>
-  <sortState ref="A2:F16">
-    <sortCondition ref="B2:B16"/>
+  <sortState ref="B2:G16">
     <sortCondition ref="C2:C16"/>
+    <sortCondition ref="D2:D16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implement query storage ui
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$21</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>Feature</t>
   </si>
@@ -160,13 +160,37 @@
     <t>Dropping a field into the filter bucket triggers a SELECT UNIQUE to get the field's values from the table. Values are available for manipulation from a right-click menu, replacing current filter interface.</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Bug: identical Value entries cause 'column ambiguously defined' (e.g. COUNTOF_ID and COUNTOF_ID in Values bucket)</t>
   </si>
   <si>
     <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value.</t>
+  </si>
+  <si>
+    <t>Logging user behavior data. Foreign key of query, and whether a chart was used (and which chart)</t>
+  </si>
+  <si>
+    <t>Display chart representation of pivot table with chart.js. Simple bar/line charts for now.</t>
+  </si>
+  <si>
+    <t>Will write a logging library that can be called with arbitrary JS objects to store information. Not sure where info will be stored. Perhaps just localstorage for now.</t>
+  </si>
+  <si>
+    <t>Add menu library to support item #s 2, 3, and context menus</t>
+  </si>
+  <si>
+    <t>Should be simple-ish assuming the output of datasource.php is suitable for charting library?</t>
+  </si>
+  <si>
+    <t>Cancelled in favour of using JQueryUI's modal dialog() for #2, and expanding contextmenu.js library for #3</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -217,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -274,6 +298,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -742,10 +769,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,10 +783,11 @@
     <col min="4" max="4" width="12.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="74.28515625" style="9" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>40</v>
       </c>
@@ -778,8 +806,14 @@
       <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="13" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="G1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -799,7 +833,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="51" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -816,10 +850,16 @@
         <v>31</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="G3" s="20">
+        <v>42964</v>
+      </c>
+      <c r="H3" s="20">
+        <v>42976</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -839,7 +879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -859,7 +899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -878,8 +918,14 @@
       <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="20">
+        <v>42965</v>
+      </c>
+      <c r="H6" s="20">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -898,8 +944,14 @@
       <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="20">
+        <v>42965</v>
+      </c>
+      <c r="H7" s="20">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -918,8 +970,14 @@
       <c r="F8" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="20">
+        <v>42965</v>
+      </c>
+      <c r="H8" s="20">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -938,8 +996,14 @@
       <c r="F9" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="G9" s="20">
+        <v>42965</v>
+      </c>
+      <c r="H9" s="20">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -959,7 +1023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -978,8 +1042,14 @@
       <c r="F11" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="G11" s="20">
+        <v>42965</v>
+      </c>
+      <c r="H11" s="20">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -999,7 +1069,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1019,7 +1089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1038,8 +1108,14 @@
       <c r="F14" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="G14" s="20">
+        <v>42965</v>
+      </c>
+      <c r="H14" s="20">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1059,7 +1135,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1079,7 +1155,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1099,12 +1175,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>4</v>
@@ -1113,17 +1189,82 @@
         <v>6</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="20">
+        <v>42965</v>
+      </c>
+      <c r="H21" s="20">
+        <v>42974</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F17">
+  <autoFilter ref="A1:F21">
     <filterColumn colId="5">
       <filters>
-        <filter val="In progress"/>
         <filter val="Not Started"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
charting improvements + cleanup
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>Feature</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Revisit UX for double-click UI operations</t>
   </si>
   <si>
-    <t>To make the UI as discoverable as possible, should 'removal' operations currently mapped to double-click instead live within right-click menus? How about an on-hover 'X' button for removing fields?</t>
-  </si>
-  <si>
     <t>This is no problem on the back end. Just need to adjust front-end validation to allow duplicate field in Values bucket</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>Fix 'column ambiguously defined' when aliasing long column values with aggregate fns</t>
   </si>
   <si>
-    <t>Look at deprecated column aliasing function. Take longest aggregate alias into account. Can these names be made more friendly? Or perhaps add metadata to the response so client can insert pretty column names?</t>
-  </si>
-  <si>
     <t>Took this to mean 'only value(s) are selected'. Add logic to validation that does not reject this query configuration. This type of query will present a single row, COUNT(*).</t>
   </si>
   <si>
@@ -160,27 +154,21 @@
     <t>Dropping a field into the filter bucket triggers a SELECT UNIQUE to get the field's values from the table. Values are available for manipulation from a right-click menu, replacing current filter interface.</t>
   </si>
   <si>
+    <t>In progress</t>
+  </si>
+  <si>
     <t>Bug: identical Value entries cause 'column ambiguously defined' (e.g. COUNTOF_ID and COUNTOF_ID in Values bucket)</t>
   </si>
   <si>
-    <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value.</t>
-  </si>
-  <si>
     <t>Logging user behavior data. Foreign key of query, and whether a chart was used (and which chart)</t>
   </si>
   <si>
     <t>Display chart representation of pivot table with chart.js. Simple bar/line charts for now.</t>
   </si>
   <si>
-    <t>Will write a logging library that can be called with arbitrary JS objects to store information. Not sure where info will be stored. Perhaps just localstorage for now.</t>
-  </si>
-  <si>
     <t>Add menu library to support item #s 2, 3, and context menus</t>
   </si>
   <si>
-    <t>Should be simple-ish assuming the output of datasource.php is suitable for charting library?</t>
-  </si>
-  <si>
     <t>Cancelled in favour of using JQueryUI's modal dialog() for #2, and expanding contextmenu.js library for #3</t>
   </si>
   <si>
@@ -191,13 +179,28 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Replace double-click delete actions with an on-hover 'X' button for removing fields.</t>
+  </si>
+  <si>
+    <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value. Will work best if end user never sees column aliases (see #11)</t>
+  </si>
+  <si>
+    <t>Will write a logging library that can be called with arbitrary JS objects to store information. How to generate &amp; track user IDs?</t>
+  </si>
+  <si>
+    <t>Alias column/reducer names to compact representation and provide hydration metadata with results object (e.g. " '2017'_COUNT_ID " &lt;=&gt; "FHD$#$PIK$#$MNA"). Both pivot table and charting lib can use rehydration to represent column names in a friendly way.</t>
+  </si>
+  <si>
+    <t>Some data contortion required. Array of arrays not supported in the case of multiple aggregators. Also, what about case of non-numeric fields? (Labels will be improved with #11)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +217,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -241,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -256,12 +267,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -271,12 +276,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -285,15 +284,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -301,6 +291,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -771,8 +797,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,64 +807,65 @@
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="74.28515625" style="7" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="G1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="51" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -846,16 +873,16 @@
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>31</v>
+      <c r="E3" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="20">
+        <v>32</v>
+      </c>
+      <c r="G3" s="13">
         <v>42964</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="13">
         <v>42976</v>
       </c>
     </row>
@@ -863,48 +890,50 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="C4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="D5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -912,17 +941,17 @@
       <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>26</v>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="20">
-        <v>42965</v>
-      </c>
-      <c r="H6" s="20">
-        <v>42965</v>
+        <v>32</v>
+      </c>
+      <c r="G6" s="13">
+        <v>42972</v>
+      </c>
+      <c r="H6" s="13">
+        <v>42972</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -938,21 +967,21 @@
       <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>24</v>
+      <c r="E7" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="20">
-        <v>42965</v>
-      </c>
-      <c r="H7" s="20">
-        <v>42965</v>
+        <v>32</v>
+      </c>
+      <c r="G7" s="13">
+        <v>42972</v>
+      </c>
+      <c r="H7" s="13">
+        <v>42972</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -964,16 +993,16 @@
       <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>39</v>
+      <c r="E8" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="20">
+        <v>32</v>
+      </c>
+      <c r="G8" s="13">
         <v>42965</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="13">
         <v>42965</v>
       </c>
     </row>
@@ -982,49 +1011,50 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="20">
-        <v>42965</v>
-      </c>
-      <c r="H9" s="20">
-        <v>42965</v>
+        <v>32</v>
+      </c>
+      <c r="G9" s="13">
+        <v>42975</v>
+      </c>
+      <c r="H9" s="13">
+        <v>42975</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="D10" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1036,61 +1066,65 @@
       <c r="D11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="20">
+        <v>32</v>
+      </c>
+      <c r="G11" s="13">
         <v>42965</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="13">
         <v>42965</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="25">
+        <v>42976</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="C13" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="F13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1102,16 +1136,16 @@
       <c r="D14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="20">
+        <v>32</v>
+      </c>
+      <c r="G14" s="13">
         <v>42965</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="13">
         <v>42965</v>
       </c>
     </row>
@@ -1119,128 +1153,136 @@
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="C15" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="C16" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="F16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="23"/>
+    </row>
+    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="25">
+        <v>42976</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="B20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -1248,16 +1290,16 @@
       <c r="D21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>50</v>
+      <c r="E21" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="20">
+        <v>47</v>
+      </c>
+      <c r="G21" s="13">
         <v>42965</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="13">
         <v>42974</v>
       </c>
     </row>
@@ -1265,6 +1307,7 @@
   <autoFilter ref="A1:F21">
     <filterColumn colId="5">
       <filters>
+        <filter val="In progress"/>
         <filter val="Not Started"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
basic charts up and running
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$23</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
   <si>
     <t>Feature</t>
   </si>
@@ -169,9 +169,6 @@
     <t>Add menu library to support item #s 2, 3, and context menus</t>
   </si>
   <si>
-    <t>Cancelled in favour of using JQueryUI's modal dialog() for #2, and expanding contextmenu.js library for #3</t>
-  </si>
-  <si>
     <t>Cancelled</t>
   </si>
   <si>
@@ -194,6 +191,39 @@
   </si>
   <si>
     <t>Some data contortion required. Array of arrays not supported in the case of multiple aggregators. Also, what about case of non-numeric fields? (Labels will be improved with #11)</t>
+  </si>
+  <si>
+    <t>Cancelled in favour of using JQueryUI's modal dialog() for #2 and #18, and expanding contextmenu.js library for #3</t>
+  </si>
+  <si>
+    <t>Refine presentation of charts, building on #18</t>
+  </si>
+  <si>
+    <t>Add toast notifications</t>
+  </si>
+  <si>
+    <t>Modals are not the best way to present chart information. Need improvements to chart visuals: sort entires respecting numeric columns (but see #11), make bar charts more legible. Is basic presentation even in line with stakeholder expectations?</t>
+  </si>
+  <si>
+    <t>Changes in pivot table shape (e.g. removing rows/cols/resorting) should be reflected in charts</t>
+  </si>
+  <si>
+    <t>Changes currently modify DOM, not app state. Conversely, charts are generated from state (specifically most recently received pivot results). Need to pin shape modifications to state.</t>
+  </si>
+  <si>
+    <t>Arrange table fields and sorting buckets in vertical stack</t>
+  </si>
+  <si>
+    <t>Restyle app for cohesive look and feel</t>
+  </si>
+  <si>
+    <t>Bootstrap would be easiest &amp; most flexible?</t>
+  </si>
+  <si>
+    <t>Combine container divs.</t>
+  </si>
+  <si>
+    <t>Toasts will give users feedback about the following: saving a query, trying to show a chart with no mostRecentResults value, successfully loaded pivot, etc. JQueryUI does not have a native toast widget.</t>
   </si>
 </sst>
 </file>
@@ -252,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -267,18 +297,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -288,9 +312,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -794,11 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,44 +827,44 @@
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="74.28515625" style="6" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>26</v>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>5</v>
@@ -852,465 +872,587 @@
       <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>27</v>
+      <c r="E2" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:8" ht="51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="22">
         <v>42964</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="22">
         <v>42976</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="22">
+        <v>42972</v>
+      </c>
+      <c r="H5" s="22">
+        <v>42972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="22">
+        <v>42972</v>
+      </c>
+      <c r="H6" s="22">
+        <v>42972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="22">
+        <v>42976</v>
+      </c>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="22">
+        <v>42965</v>
+      </c>
+      <c r="H8" s="22">
+        <v>42974</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="22">
+        <v>42975</v>
+      </c>
+      <c r="H9" s="22">
+        <v>42975</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="22">
+        <v>42976</v>
+      </c>
+      <c r="H10" s="22">
+        <v>42977</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="22">
+        <v>42965</v>
+      </c>
+      <c r="H11" s="22">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>9</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="22" t="s">
+      <c r="B12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="D13" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="24"/>
-    </row>
-    <row r="6" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="22">
+        <v>42965</v>
+      </c>
+      <c r="H14" s="22">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="22">
+        <v>42965</v>
+      </c>
+      <c r="H16" s="22">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>15</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>22</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>19</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+    </row>
+    <row r="24" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="B25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="D25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
         <v>25</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="13">
-        <v>42972</v>
-      </c>
-      <c r="H6" s="13">
-        <v>42972</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="B26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="13">
-        <v>42972</v>
-      </c>
-      <c r="H7" s="13">
-        <v>42972</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="13">
-        <v>42965</v>
-      </c>
-      <c r="H8" s="13">
-        <v>42965</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="13">
-        <v>42975</v>
-      </c>
-      <c r="H9" s="13">
-        <v>42975</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="D26" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="23"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="13">
-        <v>42965</v>
-      </c>
-      <c r="H11" s="13">
-        <v>42965</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="25">
-        <v>42976</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="23"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="13">
-        <v>42965</v>
-      </c>
-      <c r="H14" s="13">
-        <v>42965</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="23"/>
-    </row>
-    <row r="16" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="24"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="25">
-        <v>42976</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="23"/>
-    </row>
-    <row r="21" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="13">
-        <v>42965</v>
-      </c>
-      <c r="H21" s="13">
-        <v>42974</v>
-      </c>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F21">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="In progress"/>
-        <filter val="Not Started"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:H23">
+    <sortState ref="A2:H23">
+      <sortCondition ref="C2:C23"/>
+      <sortCondition ref="D2:D23"/>
+    </sortState>
   </autoFilter>
   <sortState ref="B2:G16">
     <sortCondition ref="C2:C16"/>

</xml_diff>

<commit_message>
remove double-click-to-delete in favour of delete button
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$26</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -88,9 +88,6 @@
     <t>Add logic to validation that does not reject this query configuration. This type of query will present a single row, COUNT(*) pivoted against SELECT DISTINCT column values.</t>
   </si>
   <si>
-    <t>Can re-use logic from column removal/storage. Presents a good opportunity to clean up the UI for row/column storage.</t>
-  </si>
-  <si>
     <t>Research: Can we reconstruct post-query client side adjustements to the pivot table, such as removing/renaming fields, when retrieving previous queries?</t>
   </si>
   <si>
@@ -178,18 +175,12 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Replace double-click delete actions with an on-hover 'X' button for removing fields.</t>
-  </si>
-  <si>
     <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value. Will work best if end user never sees column aliases (see #11)</t>
   </si>
   <si>
     <t>Will write a logging library that can be called with arbitrary JS objects to store information. How to generate &amp; track user IDs?</t>
   </si>
   <si>
-    <t>Alias column/reducer names to compact representation and provide hydration metadata with results object (e.g. " '2017'_COUNT_ID " &lt;=&gt; "FHD$#$PIK$#$MNA"). Both pivot table and charting lib can use rehydration to represent column names in a friendly way.</t>
-  </si>
-  <si>
     <t>Some data contortion required. Array of arrays not supported in the case of multiple aggregators. Also, what about case of non-numeric fields? (Labels will be improved with #11)</t>
   </si>
   <si>
@@ -208,9 +199,6 @@
     <t>Changes in pivot table shape (e.g. removing rows/cols/resorting) should be reflected in charts</t>
   </si>
   <si>
-    <t>Changes currently modify DOM, not app state. Conversely, charts are generated from state (specifically most recently received pivot results). Need to pin shape modifications to state.</t>
-  </si>
-  <si>
     <t>Arrange table fields and sorting buckets in vertical stack</t>
   </si>
   <si>
@@ -224,6 +212,18 @@
   </si>
   <si>
     <t>Toasts will give users feedback about the following: saving a query, trying to show a chart with no mostRecentResults value, successfully loaded pivot, etc. JQueryUI does not have a native toast widget.</t>
+  </si>
+  <si>
+    <t>Replace double-click delete actions with an on-hover 'X' button for removing fields. Use Jquery hover()</t>
+  </si>
+  <si>
+    <t>Changes currently modify DOM, not app state. Conversely, charts are generated from state (specifically most recently received pivot results). Need to pin shape modifications to state. See #11</t>
+  </si>
+  <si>
+    <t>Alias column/reducer names to compact representation and provide hydration metadata with results object (e.g. " '2017'_COUNT_ID " &lt;=&gt; "FHD$#$PIK$#$MNA"). Both pivot table and charting lib can use rehydration to represent column names in a friendly way. Perhaps pivot data should be represented as an array of cells that know their own coordinates, as in reference pivot library.</t>
+  </si>
+  <si>
+    <t>Can re-use logic from column removal/storage. Presents a good opportunity to clean up the UI for row/column storage. See #11</t>
   </si>
 </sst>
 </file>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +835,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>1</v>
@@ -853,10 +853,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -873,10 +873,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -886,7 +886,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>5</v>
@@ -895,10 +895,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="22">
         <v>42964</v>
@@ -912,19 +912,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -943,10 +943,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="22">
         <v>42972</v>
@@ -960,7 +960,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>5</v>
@@ -969,10 +969,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="22">
         <v>42972</v>
@@ -981,24 +981,24 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" s="22">
         <v>42976</v>
@@ -1010,19 +1010,19 @@
         <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>46</v>
       </c>
       <c r="G8" s="22">
         <v>42965</v>
@@ -1036,19 +1036,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="F9" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="22">
         <v>42975</v>
@@ -1062,7 +1062,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>5</v>
@@ -1071,10 +1071,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="22">
         <v>42976</v>
@@ -1097,10 +1097,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="22">
         <v>42965</v>
@@ -1123,10 +1123,10 @@
         <v>5</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -1136,7 +1136,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>4</v>
@@ -1145,10 +1145,10 @@
         <v>5</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
@@ -1170,7 +1170,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="22">
         <v>42965</v>
@@ -1184,7 +1184,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>4</v>
@@ -1193,10 +1193,10 @@
         <v>6</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -1218,7 +1218,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="22">
         <v>42965</v>
@@ -1241,10 +1241,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -1266,7 +1266,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -1285,10 +1285,10 @@
         <v>6</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
@@ -1298,7 +1298,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>6</v>
@@ -1307,42 +1307,46 @@
         <v>6</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>16</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+        <v>31</v>
+      </c>
+      <c r="G21" s="22">
+        <v>42978</v>
+      </c>
+      <c r="H21" s="22">
+        <v>42978</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>6</v>
@@ -1351,10 +1355,10 @@
         <v>6</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -1364,7 +1368,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>6</v>
@@ -1373,10 +1377,10 @@
         <v>6</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -1386,7 +1390,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>6</v>
@@ -1395,10 +1399,10 @@
         <v>5</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -1408,7 +1412,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>4</v>
@@ -1417,10 +1421,10 @@
         <v>4</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -1430,7 +1434,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>4</v>
@@ -1439,21 +1443,16 @@
         <v>6</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H23">
-    <sortState ref="A2:H23">
-      <sortCondition ref="C2:C23"/>
-      <sortCondition ref="D2:D23"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:H26"/>
   <sortState ref="B2:G16">
     <sortCondition ref="C2:C16"/>
     <sortCondition ref="D2:D16"/>

</xml_diff>

<commit_message>
ui refactor to match excel idioms
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -205,9 +205,6 @@
     <t>Restyle app for cohesive look and feel</t>
   </si>
   <si>
-    <t>Bootstrap would be easiest &amp; most flexible?</t>
-  </si>
-  <si>
     <t>Combine container divs.</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>Can re-use logic from column removal/storage. Presents a good opportunity to clean up the UI for row/column storage. See #11</t>
+  </si>
+  <si>
+    <t>Redid UI to more closely match Excel ribbon idioms. Used bootstrap for element styles. Still need to peg loading UI to toolbar element.</t>
   </si>
 </sst>
 </file>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>40</v>
@@ -1241,7 +1241,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>27</v>
@@ -1329,7 +1329,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>31</v>
@@ -1355,7 +1355,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>27</v>
@@ -1399,7 +1399,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>27</v>
@@ -1421,15 +1421,19 @@
         <v>4</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="G25" s="22">
+        <v>42979</v>
+      </c>
+      <c r="H25" s="22">
+        <v>42979</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>25</v>
       </c>
@@ -1443,12 +1447,14 @@
         <v>6</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="G26" s="22">
+        <v>42979</v>
+      </c>
       <c r="H26" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move loading indicator to toolbar
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -223,7 +223,7 @@
     <t>Can re-use logic from column removal/storage. Presents a good opportunity to clean up the UI for row/column storage. See #11</t>
   </si>
   <si>
-    <t>Redid UI to more closely match Excel ribbon idioms. Used bootstrap for element styles. Still need to peg loading UI to toolbar element.</t>
+    <t>Redid UI to more closely match Excel ribbon idioms. Used bootstrap for element styles.</t>
   </si>
 </sst>
 </file>
@@ -818,7 +818,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,7 +1433,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>25</v>
       </c>
@@ -1450,12 +1450,14 @@
         <v>64</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G26" s="22">
         <v>42979</v>
       </c>
-      <c r="H26" s="20"/>
+      <c r="H26" s="22">
+        <v>42984</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H26"/>

</xml_diff>

<commit_message>
load status ui and halting pending responses
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,10 +1266,14 @@
         <v>14</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+        <v>31</v>
+      </c>
+      <c r="G18" s="22">
+        <v>42984</v>
+      </c>
+      <c r="H18" s="22">
+        <v>42984</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="16">

</xml_diff>

<commit_message>
express_data working for row coords.
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
   <si>
     <t>Feature</t>
   </si>
@@ -193,9 +193,6 @@
     <t>Add toast notifications</t>
   </si>
   <si>
-    <t>Modals are not the best way to present chart information. Need improvements to chart visuals: sort entires respecting numeric columns (but see #11), make bar charts more legible. Is basic presentation even in line with stakeholder expectations?</t>
-  </si>
-  <si>
     <t>Changes in pivot table shape (e.g. removing rows/cols/resorting) should be reflected in charts</t>
   </si>
   <si>
@@ -217,20 +214,35 @@
     <t>Changes currently modify DOM, not app state. Conversely, charts are generated from state (specifically most recently received pivot results). Need to pin shape modifications to state. See #11</t>
   </si>
   <si>
-    <t>Alias column/reducer names to compact representation and provide hydration metadata with results object (e.g. " '2017'_COUNT_ID " &lt;=&gt; "FHD$#$PIK$#$MNA"). Both pivot table and charting lib can use rehydration to represent column names in a friendly way. Perhaps pivot data should be represented as an array of cells that know their own coordinates, as in reference pivot library.</t>
-  </si>
-  <si>
     <t>Can re-use logic from column removal/storage. Presents a good opportunity to clean up the UI for row/column storage. See #11</t>
   </si>
   <si>
     <t>Redid UI to more closely match Excel ribbon idioms. Used bootstrap for element styles.</t>
+  </si>
+  <si>
+    <t>Allow user to toggle live fetching of pivot data from server</t>
+  </si>
+  <si>
+    <t>Flag will bypass call to sendConfig() in pivotController.js</t>
+  </si>
+  <si>
+    <t>Need improvements to chart visuals: sort entires respecting numeric columns (but see #11), make bar charts more legible. Legends take up too much space at bottom of chart. Can charts be resized?</t>
+  </si>
+  <si>
+    <t>Save/load should be keyed, not array of models</t>
+  </si>
+  <si>
+    <t>Give saved models an ID, so that new saves can overwrite current 'file' or else do a 'save as…'</t>
+  </si>
+  <si>
+    <t>Alias column/reducer names to compact representation and provide hydration metadata with results object (e.g. " '2017'_COUNT_ID " &lt;=&gt; "FHD$#$PIK$#$MNA"). Both pivot table and charting lib can use rehydration to represent column names in a friendly way. Perhaps pivot data should be represented a hash of cells that know their own coordinates, as in reference pivot library.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,14 +259,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -305,50 +309,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,10 +819,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,77 +832,78 @@
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="79.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-    </row>
-    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G3" s="22">
@@ -907,45 +913,45 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="C4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>6</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G5" s="22">
@@ -955,23 +961,23 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="22">
@@ -981,47 +987,47 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="C7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>40</v>
       </c>
       <c r="G7" s="22">
         <v>42976</v>
       </c>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="C8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="22">
@@ -1031,23 +1037,23 @@
         <v>42974</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="C9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="22">
@@ -1057,23 +1063,23 @@
         <v>42975</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
         <v>18</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="C10" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G10" s="22">
@@ -1083,189 +1089,189 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="11">
         <v>42965</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="11">
         <v>42965</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+    <row r="12" spans="1:8" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
         <v>9</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
         <v>4</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="11">
         <v>42965</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="11">
         <v>42965</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <v>17</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="1:8" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" s="8" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="11">
         <v>42965</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="11">
         <v>42965</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
         <v>14</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="16" t="s">
+      <c r="C17" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
         <v>12</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="C18" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G18" s="22">
@@ -1275,67 +1281,67 @@
         <v>42984</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
         <v>15</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="9" t="s">
+      <c r="C19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-    </row>
-    <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
         <v>21</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="16" t="s">
+      <c r="C20" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
         <v>16</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="16" t="s">
+      <c r="C21" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="16" t="s">
+      <c r="E21" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G21" s="22">
@@ -1345,89 +1351,89 @@
         <v>42978</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
         <v>22</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="16" t="s">
+      <c r="C22" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-    </row>
-    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
         <v>19</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="C23" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>24</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="16" t="s">
+      <c r="E25" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G25" s="22">
@@ -1437,23 +1443,23 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="15" t="s">
+      <c r="B26" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="16" t="s">
+      <c r="D26" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G26" s="22">
@@ -1463,8 +1469,62 @@
         <v>42984</v>
       </c>
     </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>26</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H26"/>
+  <autoFilter ref="A1:H26">
+    <filterColumn colId="7">
+      <filters blank="1">
+        <dateGroupItem year="2017" month="8" day="25" dateTimeGrouping="day"/>
+        <dateGroupItem year="2017" month="8" day="27" dateTimeGrouping="day"/>
+        <dateGroupItem year="2017" month="8" day="28" dateTimeGrouping="day"/>
+        <dateGroupItem year="2017" month="8" day="29" dateTimeGrouping="day"/>
+        <dateGroupItem year="2017" month="8" day="30" dateTimeGrouping="day"/>
+        <dateGroupItem year="2017" month="8" day="31" dateTimeGrouping="day"/>
+        <dateGroupItem year="2017" month="9" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="B2:G16">
     <sortCondition ref="C2:C16"/>
     <sortCondition ref="D2:D16"/>

</xml_diff>

<commit_message>
correctly render table with all combos of >0/0 cols/aggs
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18555" windowHeight="4830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$28</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -151,9 +151,6 @@
     <t>Dropping a field into the filter bucket triggers a SELECT UNIQUE to get the field's values from the table. Values are available for manipulation from a right-click menu, replacing current filter interface.</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Bug: identical Value entries cause 'column ambiguously defined' (e.g. COUNTOF_ID and COUNTOF_ID in Values bucket)</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value. Will work best if end user never sees column aliases (see #11)</t>
-  </si>
-  <si>
     <t>Will write a logging library that can be called with arbitrary JS objects to store information. How to generate &amp; track user IDs?</t>
   </si>
   <si>
@@ -236,6 +230,12 @@
   </si>
   <si>
     <t>Alias column/reducer names to compact representation and provide hydration metadata with results object (e.g. " '2017'_COUNT_ID " &lt;=&gt; "FHD$#$PIK$#$MNA"). Both pivot table and charting lib can use rehydration to represent column names in a friendly way. Perhaps pivot data should be represented a hash of cells that know their own coordinates, as in reference pivot library.</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value. Will work best if end user never sees column aliases (current implementation of #11 doesn't deal with this, but it can be accommodated by creating different aliases if the request to register an alias came from an aggregator fn.)</t>
   </si>
 </sst>
 </file>
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -352,6 +352,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -822,8 +825,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,10 +862,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -887,7 +890,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -935,7 +938,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>6</v>
       </c>
@@ -961,7 +964,7 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -987,7 +990,7 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>11</v>
       </c>
@@ -1001,34 +1004,36 @@
         <v>5</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G7" s="22">
         <v>42976</v>
       </c>
-      <c r="H7" s="18"/>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" s="23">
+        <v>42992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>20</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="G8" s="22">
         <v>42965</v>
@@ -1037,7 +1042,7 @@
         <v>42974</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -1063,12 +1068,12 @@
         <v>42975</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>18</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>5</v>
@@ -1077,7 +1082,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>31</v>
@@ -1154,9 +1159,11 @@
         <v>30</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="G13" s="23">
+        <v>42990</v>
+      </c>
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
@@ -1185,12 +1192,12 @@
         <v>42965</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>17</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>4</v>
@@ -1199,7 +1206,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>27</v>
@@ -1247,7 +1254,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>27</v>
@@ -1255,7 +1262,7 @@
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
     </row>
-    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>12</v>
       </c>
@@ -1308,7 +1315,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>6</v>
@@ -1317,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>27</v>
@@ -1325,7 +1332,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>16</v>
       </c>
@@ -1339,7 +1346,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>31</v>
@@ -1356,7 +1363,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>6</v>
@@ -1365,7 +1372,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>27</v>
@@ -1378,7 +1385,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>6</v>
@@ -1387,7 +1394,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>27</v>
@@ -1400,7 +1407,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>6</v>
@@ -1409,7 +1416,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>27</v>
@@ -1417,12 +1424,12 @@
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>4</v>
@@ -1431,7 +1438,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>31</v>
@@ -1443,12 +1450,12 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>4</v>
@@ -1457,7 +1464,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>31</v>
@@ -1474,7 +1481,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>4</v>
@@ -1483,7 +1490,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>27</v>
@@ -1496,7 +1503,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>6</v>
@@ -1505,23 +1512,18 @@
         <v>6</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H26">
-    <filterColumn colId="7">
-      <filters blank="1">
-        <dateGroupItem year="2017" month="8" day="25" dateTimeGrouping="day"/>
-        <dateGroupItem year="2017" month="8" day="27" dateTimeGrouping="day"/>
-        <dateGroupItem year="2017" month="8" day="28" dateTimeGrouping="day"/>
-        <dateGroupItem year="2017" month="8" day="29" dateTimeGrouping="day"/>
-        <dateGroupItem year="2017" month="8" day="30" dateTimeGrouping="day"/>
-        <dateGroupItem year="2017" month="8" day="31" dateTimeGrouping="day"/>
-        <dateGroupItem year="2017" month="9" dateTimeGrouping="month"/>
+  <autoFilter ref="A1:H28">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="In Progress"/>
+        <filter val="Not Started"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
add charting for expressive results
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -825,8 +825,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,10 +1257,14 @@
         <v>59</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="G17" s="22">
+        <v>42996</v>
+      </c>
+      <c r="H17" s="22">
+        <v>42996</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
@@ -1419,10 +1423,14 @@
         <v>58</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="G24" s="22">
+        <v>42996</v>
+      </c>
+      <c r="H24" s="22">
+        <v>42996</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
@@ -1508,10 +1516,10 @@
       <c r="C28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="D28" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>65</v>
       </c>
       <c r="F28" s="4" t="s">

</xml_diff>

<commit_message>
cleanups to make way for save as queries
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -91,9 +91,6 @@
     <t>Research: Can we reconstruct post-query client side adjustements to the pivot table, such as removing/renaming fields, when retrieving previous queries?</t>
   </si>
   <si>
-    <t>Easy to rename table cells. Can't remember what is meant by 'dropdowns are best'.</t>
-  </si>
-  <si>
     <t>Revisit UX for double-click UI operations</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value. Will work best if end user never sees column aliases (current implementation of #11 doesn't deal with this, but it can be accommodated by creating different aliases if the request to register an alias came from an aggregator fn.)</t>
+  </si>
+  <si>
+    <t>Will register a new transform for remapping.</t>
   </si>
 </sst>
 </file>
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -355,6 +355,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -825,8 +828,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +847,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -853,7 +856,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>1</v>
@@ -862,10 +865,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -882,10 +885,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -895,7 +898,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>5</v>
@@ -904,10 +907,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="22">
         <v>42964</v>
@@ -921,19 +924,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -952,10 +955,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="22">
         <v>42972</v>
@@ -969,7 +972,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>5</v>
@@ -978,10 +981,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="22">
         <v>42972</v>
@@ -995,7 +998,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>5</v>
@@ -1004,10 +1007,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="22">
         <v>42976</v>
@@ -1021,19 +1024,19 @@
         <v>20</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>44</v>
       </c>
       <c r="G8" s="22">
         <v>42965</v>
@@ -1047,19 +1050,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="F9" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="22">
         <v>42975</v>
@@ -1073,7 +1076,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>5</v>
@@ -1082,10 +1085,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="22">
         <v>42976</v>
@@ -1108,10 +1111,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="11">
         <v>42965</v>
@@ -1134,10 +1137,10 @@
         <v>5</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -1156,15 +1159,17 @@
         <v>5</v>
       </c>
       <c r="E13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>67</v>
       </c>
       <c r="G13" s="23">
         <v>42990</v>
       </c>
-      <c r="H13" s="18"/>
+      <c r="H13" s="23">
+        <v>42999</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -1183,7 +1188,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="11">
         <v>42965</v>
@@ -1197,7 +1202,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>4</v>
@@ -1206,10 +1211,10 @@
         <v>6</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -1231,7 +1236,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" s="11">
         <v>42965</v>
@@ -1254,10 +1259,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="22">
         <v>42996</v>
@@ -1283,7 +1288,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="22">
         <v>42984</v>
@@ -1306,10 +1311,10 @@
         <v>6</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
@@ -1319,7 +1324,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>6</v>
@@ -1328,10 +1333,10 @@
         <v>6</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
@@ -1341,7 +1346,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>6</v>
@@ -1350,10 +1355,10 @@
         <v>4</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="22">
         <v>42978</v>
@@ -1367,7 +1372,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>6</v>
@@ -1376,10 +1381,10 @@
         <v>6</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -1389,7 +1394,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>6</v>
@@ -1398,10 +1403,10 @@
         <v>6</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -1411,7 +1416,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>6</v>
@@ -1420,10 +1425,10 @@
         <v>5</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="22">
         <v>42996</v>
@@ -1437,7 +1442,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>4</v>
@@ -1446,10 +1451,10 @@
         <v>4</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25" s="22">
         <v>42979</v>
@@ -1463,7 +1468,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>4</v>
@@ -1472,10 +1477,10 @@
         <v>6</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" s="22">
         <v>42979</v>
@@ -1489,7 +1494,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>4</v>
@@ -1498,10 +1503,10 @@
         <v>4</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -1511,19 +1516,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>65</v>
-      </c>
       <c r="F28" s="4" t="s">
-        <v>27</v>
+        <v>66</v>
+      </c>
+      <c r="G28" s="24">
+        <v>42999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update/save new for specific saved queries
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
   <si>
     <t>Feature</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>Alias column/reducer names to compact representation and provide hydration metadata with results object (e.g. " '2017'_COUNT_ID " &lt;=&gt; "FHD$#$PIK$#$MNA"). Both pivot table and charting lib can use rehydration to represent column names in a friendly way. Perhaps pivot data should be represented a hash of cells that know their own coordinates, as in reference pivot library.</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value. Will work best if end user never sees column aliases (current implementation of #11 doesn't deal with this, but it can be accommodated by creating different aliases if the request to register an alias came from an aggregator fn.)</t>
@@ -825,11 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +889,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -941,7 +937,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>6</v>
       </c>
@@ -967,7 +963,7 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -993,7 +989,7 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>11</v>
       </c>
@@ -1019,7 +1015,7 @@
         <v>42992</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>20</v>
       </c>
@@ -1045,7 +1041,7 @@
         <v>42974</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -1071,7 +1067,7 @@
         <v>42975</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>18</v>
       </c>
@@ -1097,7 +1093,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>7</v>
       </c>
@@ -1171,7 +1167,7 @@
         <v>42999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>10</v>
       </c>
@@ -1211,7 +1207,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>26</v>
@@ -1219,7 +1215,7 @@
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:8" s="8" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>13</v>
       </c>
@@ -1271,7 +1267,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>12</v>
       </c>
@@ -1311,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>26</v>
@@ -1341,7 +1337,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>16</v>
       </c>
@@ -1437,7 +1433,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -1463,7 +1459,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -1528,21 +1524,17 @@
         <v>64</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="G28" s="24">
         <v>42999</v>
       </c>
+      <c r="H28" s="24">
+        <v>42999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H28">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="In Progress"/>
-        <filter val="Not Started"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H28"/>
   <sortState ref="B2:G16">
     <sortCondition ref="C2:C16"/>
     <sortCondition ref="D2:D16"/>

</xml_diff>

<commit_message>
pull down external css/js deps
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$29</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="73">
   <si>
     <t>Feature</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Query information is already being updated in lockstep with user actions. Trivial to store query objects (in localstorage to start with). On retrieval, fire off the stored query object and rearrange selection bucket DOM to match object. DOM arrangement will require rewriting some code in client-side View module.</t>
   </si>
   <si>
-    <t>Possibly. Best guess is to maintain an object describing transformations made to the 'base' pivot table returned from server, then applying transformations to a fresh copy of that query/table in a sensible order. There are a huge number of possible transformations that a user can make to the table, so this will be difficult to get 100% correct. Also we are concerned that this approach may not scale for future ways of displaying pivot table results.</t>
-  </si>
-  <si>
     <t>Complete</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>Changes currently modify DOM, not app state. Conversely, charts are generated from state (specifically most recently received pivot results). Need to pin shape modifications to state. See #11</t>
   </si>
   <si>
-    <t>Can re-use logic from column removal/storage. Presents a good opportunity to clean up the UI for row/column storage. See #11</t>
-  </si>
-  <si>
     <t>Redid UI to more closely match Excel ribbon idioms. Used bootstrap for element styles.</t>
   </si>
   <si>
@@ -220,19 +214,40 @@
     <t>Need improvements to chart visuals: sort entires respecting numeric columns (but see #11), make bar charts more legible. Legends take up too much space at bottom of chart. Can charts be resized?</t>
   </si>
   <si>
-    <t>Save/load should be keyed, not array of models</t>
-  </si>
-  <si>
     <t>Give saved models an ID, so that new saves can overwrite current 'file' or else do a 'save as…'</t>
   </si>
   <si>
-    <t>Alias column/reducer names to compact representation and provide hydration metadata with results object (e.g. " '2017'_COUNT_ID " &lt;=&gt; "FHD$#$PIK$#$MNA"). Both pivot table and charting lib can use rehydration to represent column names in a friendly way. Perhaps pivot data should be represented a hash of cells that know their own coordinates, as in reference pivot library.</t>
-  </si>
-  <si>
     <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value. Will work best if end user never sees column aliases (current implementation of #11 doesn't deal with this, but it can be accommodated by creating different aliases if the request to register an alias came from an aggregator fn.)</t>
   </si>
   <si>
     <t>Will register a new transform for remapping.</t>
+  </si>
+  <si>
+    <t>Transformations have made this possible. Transforms are included with the data saved about a query. When loaded, the transform is pulled out and combined with the pivot result when it comes back from the server.</t>
+  </si>
+  <si>
+    <t>Should be able to both 'save' and 'save as' queries</t>
+  </si>
+  <si>
+    <t>Got this for free with expressive results/transformations. See #11</t>
+  </si>
+  <si>
+    <t>On the server, alias column/reducer names to compact representation and keep hydration mappings that can be applied to the results returned from the DB. e.g. the string "2017" is replaced with random identifier "SDKJG" wherever it occurs in the query. Before passing results back to the client, replace all random identifiers with their 'real' string representations. Also allows us to represent results in a more sophisticated way than array-of-arrays. (The term for this new representation is 'expressive results')</t>
+  </si>
+  <si>
+    <t>Move jQuery and other external libs onto server</t>
+  </si>
+  <si>
+    <t>Can FontAwesome be pulled down like this?</t>
+  </si>
+  <si>
+    <t>Remove dead code from recently-changed libs</t>
+  </si>
+  <si>
+    <t>Affects tpivot and tchart</t>
+  </si>
+  <si>
+    <t>Merge utils.js and tutils.js</t>
   </si>
 </sst>
 </file>
@@ -822,10 +837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +859,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -861,10 +877,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -881,7 +897,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>26</v>
@@ -889,12 +905,12 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>5</v>
@@ -906,7 +922,7 @@
         <v>28</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="22">
         <v>42964</v>
@@ -937,7 +953,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>6</v>
       </c>
@@ -954,7 +970,7 @@
         <v>21</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="22">
         <v>42972</v>
@@ -963,7 +979,7 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -980,7 +996,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="22">
         <v>42972</v>
@@ -989,12 +1005,12 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>11</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>5</v>
@@ -1003,10 +1019,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="22">
         <v>42976</v>
@@ -1015,24 +1031,24 @@
         <v>42992</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>20</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="G8" s="22">
         <v>42965</v>
@@ -1041,24 +1057,24 @@
         <v>42974</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>32</v>
-      </c>
       <c r="F9" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="22">
         <v>42975</v>
@@ -1067,12 +1083,12 @@
         <v>42975</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>18</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>5</v>
@@ -1081,10 +1097,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="22">
         <v>42976</v>
@@ -1093,7 +1109,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>7</v>
       </c>
@@ -1107,10 +1123,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="11">
         <v>42965</v>
@@ -1133,7 +1149,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>26</v>
@@ -1141,7 +1157,7 @@
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>4</v>
       </c>
@@ -1155,10 +1171,10 @@
         <v>5</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="23">
         <v>42990</v>
@@ -1167,7 +1183,7 @@
         <v>42999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>10</v>
       </c>
@@ -1184,7 +1200,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G14" s="11">
         <v>42965</v>
@@ -1198,7 +1214,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>4</v>
@@ -1207,7 +1223,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>26</v>
@@ -1215,7 +1231,7 @@
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:8" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="8" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>13</v>
       </c>
@@ -1232,7 +1248,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="11">
         <v>42965</v>
@@ -1241,7 +1257,7 @@
         <v>42965</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>14</v>
       </c>
@@ -1255,10 +1271,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="22">
         <v>42996</v>
@@ -1267,7 +1283,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>12</v>
       </c>
@@ -1284,7 +1300,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="22">
         <v>42984</v>
@@ -1307,7 +1323,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>26</v>
@@ -1320,7 +1336,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>6</v>
@@ -1329,7 +1345,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>26</v>
@@ -1337,7 +1353,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>16</v>
       </c>
@@ -1351,10 +1367,10 @@
         <v>4</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21" s="22">
         <v>42978</v>
@@ -1368,7 +1384,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>6</v>
@@ -1377,7 +1393,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>26</v>
@@ -1390,7 +1406,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>6</v>
@@ -1399,7 +1415,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>26</v>
@@ -1407,12 +1423,12 @@
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
     </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>6</v>
@@ -1421,10 +1437,10 @@
         <v>5</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G24" s="22">
         <v>42996</v>
@@ -1433,12 +1449,12 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>4</v>
@@ -1447,10 +1463,10 @@
         <v>4</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" s="22">
         <v>42979</v>
@@ -1459,12 +1475,12 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>4</v>
@@ -1473,10 +1489,10 @@
         <v>6</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" s="22">
         <v>42979</v>
@@ -1490,7 +1506,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>4</v>
@@ -1499,7 +1515,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>26</v>
@@ -1507,24 +1523,24 @@
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G28" s="24">
         <v>42999</v>
@@ -1533,8 +1549,77 @@
         <v>42999</v>
       </c>
     </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="24">
+        <v>43003</v>
+      </c>
+      <c r="H29" s="24">
+        <v>43003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H28"/>
+  <autoFilter ref="A1:H29">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Not Started"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="B2:G16">
     <sortCondition ref="C2:C16"/>
     <sortCondition ref="D2:D16"/>

</xml_diff>

<commit_message>
break makeExpressiveTable into sub fns
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="80">
   <si>
     <t>Feature</t>
   </si>
@@ -238,16 +238,37 @@
     <t>Move jQuery and other external libs onto server</t>
   </si>
   <si>
-    <t>Can FontAwesome be pulled down like this?</t>
-  </si>
-  <si>
     <t>Remove dead code from recently-changed libs</t>
   </si>
   <si>
     <t>Affects tpivot and tchart</t>
   </si>
   <si>
-    <t>Merge utils.js and tutils.js</t>
+    <t>Drag and drop sorting for row/cols</t>
+  </si>
+  <si>
+    <t>Cols is not too bad. Need to research how to grab row headers of same depth for a sorting group</t>
+  </si>
+  <si>
+    <t>Row headers should appear hierarchical like col headers</t>
+  </si>
+  <si>
+    <t>For each included row, keep track of how many contiguous values there are for each label. When iterating through rows, only draw the label (with rowspan=contiguous) when coordinateIndex % contiguous === 0</t>
+  </si>
+  <si>
+    <t>Enumerate all external libs</t>
+  </si>
+  <si>
+    <t>Row/Col totals</t>
+  </si>
+  <si>
+    <t>Like excel pivot tables</t>
+  </si>
+  <si>
+    <t>Load discard save save as</t>
+  </si>
+  <si>
+    <t>Relabel save/load buttons</t>
   </si>
 </sst>
 </file>
@@ -838,10 +859,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,8 +1570,8 @@
         <v>42999</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+    <row r="29" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
         <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -1563,57 +1584,130 @@
         <v>4</v>
       </c>
       <c r="E29" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="22">
+        <v>43003</v>
+      </c>
+      <c r="H29" s="22">
+        <v>43003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>29</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G29" s="24">
+      <c r="C30" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="22">
         <v>43003</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H30" s="22">
         <v>43003</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="3" t="s">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>30</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>31</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>31</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="4" t="s">
+      <c r="E34" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H29">
+  <autoFilter ref="A1:H32">
     <filterColumn colId="5">
       <filters>
         <filter val="Not Started"/>

</xml_diff>

<commit_message>
relabel save/load toolbar buttons
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -70,9 +70,6 @@
     <t>Limitation - Removing Unwanted Rows</t>
   </si>
   <si>
-    <t>Ability to rename column row result values for first row /column (dropdowns are best)</t>
-  </si>
-  <si>
     <t>Each query is assigned a unique ID when it is sent to server. Client maintains a buffer of pending queries. When user signals to halt current queries, results of queries in the buffer will be discarded when they return from the server. Queries made after the 'halt' command will be treated as normal.</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>Flag will bypass call to sendConfig() in pivotController.js</t>
   </si>
   <si>
-    <t>Need improvements to chart visuals: sort entires respecting numeric columns (but see #11), make bar charts more legible. Legends take up too much space at bottom of chart. Can charts be resized?</t>
-  </si>
-  <si>
     <t>Give saved models an ID, so that new saves can overwrite current 'file' or else do a 'save as…'</t>
   </si>
   <si>
@@ -247,9 +241,6 @@
     <t>Drag and drop sorting for row/cols</t>
   </si>
   <si>
-    <t>Cols is not too bad. Need to research how to grab row headers of same depth for a sorting group</t>
-  </si>
-  <si>
     <t>Row headers should appear hierarchical like col headers</t>
   </si>
   <si>
@@ -269,6 +260,15 @@
   </si>
   <si>
     <t>Relabel save/load buttons</t>
+  </si>
+  <si>
+    <t>Ability to rename row/column/aggregator labels</t>
+  </si>
+  <si>
+    <t>Need improvements to chart visuals: sort entires respecting numeric columns (but see #11), make bar charts more legible. Legends take up too much space at bottom of chart. Can charts be resized? Do charts respect label renaming? Also, charts do not work with length 0 aggregators.</t>
+  </si>
+  <si>
+    <t>Sorting done through a dedicated UI element.</t>
   </si>
 </sst>
 </file>
@@ -861,8 +861,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +880,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -889,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>1</v>
@@ -898,10 +898,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -918,10 +918,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -931,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>5</v>
@@ -940,10 +940,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="22">
         <v>42964</v>
@@ -957,19 +957,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -988,10 +988,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="22">
         <v>42972</v>
@@ -1005,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>5</v>
@@ -1014,10 +1014,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="22">
         <v>42972</v>
@@ -1031,7 +1031,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>5</v>
@@ -1040,10 +1040,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="22">
         <v>42976</v>
@@ -1057,19 +1057,19 @@
         <v>20</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="G8" s="22">
         <v>42965</v>
@@ -1083,19 +1083,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="22">
         <v>42975</v>
@@ -1109,7 +1109,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>5</v>
@@ -1118,10 +1118,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="22">
         <v>42976</v>
@@ -1144,10 +1144,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="11">
         <v>42965</v>
@@ -1161,7 +1161,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>4</v>
@@ -1170,10 +1170,10 @@
         <v>5</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -1183,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>4</v>
@@ -1192,10 +1192,10 @@
         <v>5</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="23">
         <v>42990</v>
@@ -1218,10 +1218,10 @@
         <v>4</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="11">
         <v>42965</v>
@@ -1235,7 +1235,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>4</v>
@@ -1244,10 +1244,10 @@
         <v>6</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -1266,10 +1266,10 @@
         <v>6</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="11">
         <v>42965</v>
@@ -1292,10 +1292,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="22">
         <v>42996</v>
@@ -1309,7 +1309,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>6</v>
@@ -1318,10 +1318,10 @@
         <v>6</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="22">
         <v>42984</v>
@@ -1335,29 +1335,33 @@
         <v>15</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G19" s="23">
+        <v>43005</v>
+      </c>
+      <c r="H19" s="23">
+        <v>43006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>21</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>6</v>
@@ -1366,10 +1370,10 @@
         <v>6</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
@@ -1379,7 +1383,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>6</v>
@@ -1388,10 +1392,10 @@
         <v>4</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" s="22">
         <v>42978</v>
@@ -1405,7 +1409,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>6</v>
@@ -1414,10 +1418,10 @@
         <v>6</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -1427,7 +1431,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>6</v>
@@ -1436,10 +1440,10 @@
         <v>6</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -1449,7 +1453,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>6</v>
@@ -1458,10 +1462,10 @@
         <v>5</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G24" s="22">
         <v>42996</v>
@@ -1475,7 +1479,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>4</v>
@@ -1484,10 +1488,10 @@
         <v>4</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25" s="22">
         <v>42979</v>
@@ -1501,7 +1505,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>4</v>
@@ -1510,10 +1514,10 @@
         <v>6</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G26" s="22">
         <v>42979</v>
@@ -1527,7 +1531,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>4</v>
@@ -1536,10 +1540,10 @@
         <v>4</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -1549,7 +1553,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>6</v>
@@ -1558,10 +1562,10 @@
         <v>6</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G28" s="24">
         <v>42999</v>
@@ -1575,7 +1579,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>5</v>
@@ -1584,10 +1588,10 @@
         <v>4</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G29" s="22">
         <v>43003</v>
@@ -1601,7 +1605,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>4</v>
@@ -1610,10 +1614,10 @@
         <v>4</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30" s="22">
         <v>43003</v>
@@ -1622,12 +1626,12 @@
         <v>43003</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>5</v>
@@ -1636,20 +1640,24 @@
         <v>6</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="G31" s="23">
+        <v>43004</v>
+      </c>
+      <c r="H31" s="23">
+        <v>43005</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>5</v>
@@ -1658,20 +1666,24 @@
         <v>6</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G32" s="23">
+        <v>43004</v>
+      </c>
+      <c r="H32" s="23">
+        <v>43004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>5</v>
@@ -1679,19 +1691,19 @@
       <c r="D33" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>77</v>
+      <c r="E33" s="19" t="s">
+        <v>74</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -1699,11 +1711,17 @@
       <c r="D34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>78</v>
+      <c r="E34" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="G34" s="23">
+        <v>43006</v>
+      </c>
+      <c r="H34" s="23">
+        <v>43006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
table owner and name are parameterized
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="83">
   <si>
     <t>Feature</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Save/restore queries</t>
   </si>
   <si>
-    <t>Dropping a field into the filter bucket triggers a SELECT UNIQUE to get the field's values from the table. Values are available for manipulation from a right-click menu, replacing current filter interface.</t>
-  </si>
-  <si>
     <t>Bug: identical Value entries cause 'column ambiguously defined' (e.g. COUNTOF_ID and COUNTOF_ID in Values bucket)</t>
   </si>
   <si>
@@ -269,6 +266,18 @@
   </si>
   <si>
     <t>Sorting done through a dedicated UI element.</t>
+  </si>
+  <si>
+    <t>Dropping a field into the filter bucket triggers a SELECT UNIQUE to get the field's values from the table. Have been asked to retain SQL style queries. That code is not activated right now--need to refactor a bit before it can be readded.</t>
+  </si>
+  <si>
+    <t>Add new database location</t>
+  </si>
+  <si>
+    <t>Current DB location is somewhat hard-coded. Need to refactor some stuff to make this work.</t>
+  </si>
+  <si>
+    <t>Remove legend from graphs</t>
   </si>
 </sst>
 </file>
@@ -859,10 +868,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,10 +907,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -918,13 +927,17 @@
         <v>5</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="G2" s="23">
+        <v>43006</v>
+      </c>
+      <c r="H2" s="23">
+        <v>43006</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
@@ -1040,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>28</v>
@@ -1057,19 +1070,19 @@
         <v>20</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="G8" s="22">
         <v>42965</v>
@@ -1109,7 +1122,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>5</v>
@@ -1118,7 +1131,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>28</v>
@@ -1192,7 +1205,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>28</v>
@@ -1235,7 +1248,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>4</v>
@@ -1244,7 +1257,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>25</v>
@@ -1292,7 +1305,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>28</v>
@@ -1335,7 +1348,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>6</v>
@@ -1344,7 +1357,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>28</v>
@@ -1361,7 +1374,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>6</v>
@@ -1370,7 +1383,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>25</v>
@@ -1392,7 +1405,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>28</v>
@@ -1409,7 +1422,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>6</v>
@@ -1418,7 +1431,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>25</v>
@@ -1431,7 +1444,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>6</v>
@@ -1440,7 +1453,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>25</v>
@@ -1453,7 +1466,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>6</v>
@@ -1462,7 +1475,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>28</v>
@@ -1479,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>4</v>
@@ -1488,7 +1501,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>28</v>
@@ -1505,7 +1518,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>4</v>
@@ -1514,7 +1527,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>28</v>
@@ -1531,7 +1544,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>4</v>
@@ -1540,7 +1553,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>25</v>
@@ -1553,7 +1566,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>6</v>
@@ -1562,7 +1575,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>28</v>
@@ -1579,7 +1592,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>5</v>
@@ -1588,7 +1601,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>28</v>
@@ -1605,7 +1618,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>4</v>
@@ -1614,7 +1627,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>28</v>
@@ -1631,7 +1644,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>5</v>
@@ -1640,7 +1653,7 @@
         <v>6</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>28</v>
@@ -1657,16 +1670,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>71</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>28</v>
@@ -1682,17 +1695,17 @@
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>74</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>25</v>
@@ -1700,19 +1713,19 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>31</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>28</v>
@@ -1722,6 +1735,43 @@
       </c>
       <c r="H34" s="23">
         <v>43006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dynamic loading of DBs and contained tables
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="86">
   <si>
     <t>Feature</t>
   </si>
@@ -278,6 +278,15 @@
   </si>
   <si>
     <t>Remove legend from graphs</t>
+  </si>
+  <si>
+    <t>Ability to query ANY table from given DB</t>
+  </si>
+  <si>
+    <t>On page load, server asks DB for list of tables. Used to poplate window.availableTables.</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -868,10 +877,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1763,13 @@
         <v>81</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="G35" s="24">
+        <v>43018</v>
+      </c>
+      <c r="H35" s="24">
+        <v>43019</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1772,6 +1787,29 @@
       </c>
       <c r="F36" s="4" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="24">
+        <v>43019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct tracking of bucket values with identical names
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -205,9 +205,6 @@
     <t>Give saved models an ID, so that new saves can overwrite current 'file' or else do a 'save as…'</t>
   </si>
   <si>
-    <t>Detect whether duplication is happening, and adjust SQL query's alias for the aggregate value. Will work best if end user never sees column aliases (current implementation of #11 doesn't deal with this, but it can be accommodated by creating different aliases if the request to register an alias came from an aggregator fn.)</t>
-  </si>
-  <si>
     <t>Will register a new transform for remapping.</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>Examine sequencing of async table/retrieval fns. Do callbacks remove pivot/sortable elements? Worst case, write new fn for loading queries that incorporates table/field retrieval but without DOM destruction</t>
+  </si>
+  <si>
+    <t>Reject queries with duplicate filter signatures on server-side validation step. This just tosses the server request; there's no reason to return a query containing dupe values.</t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -999,7 +999,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>5</v>
@@ -1008,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>28</v>
@@ -1025,7 +1025,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1048,7 +1048,7 @@
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1057,7 +1057,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>28</v>
@@ -1074,7 +1074,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1083,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>28</v>
@@ -1199,34 +1199,38 @@
         <v>42965</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+    <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>17</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="C13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="13">
+        <v>43032</v>
+      </c>
+      <c r="H13" s="13">
+        <v>43032</v>
+      </c>
     </row>
     <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -1235,7 +1239,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>28</v>
@@ -1252,16 +1256,16 @@
         <v>31</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>28</v>
@@ -1278,16 +1282,16 @@
         <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="F16" s="17" t="s">
         <v>25</v>
@@ -1300,16 +1304,16 @@
         <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>28</v>
@@ -1326,16 +1330,16 @@
         <v>37</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="F18" s="17" t="s">
         <v>25</v>
@@ -1357,7 +1361,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>28</v>
@@ -1403,7 +1407,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>28</v>
@@ -1481,7 +1485,7 @@
         <v>6</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>28</v>
@@ -1524,7 +1528,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -1559,7 +1563,7 @@
         <v>6</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>25</v>
@@ -1646,7 +1650,7 @@
         <v>15</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>6</v>
@@ -1655,7 +1659,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>28</v>
@@ -1724,7 +1728,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
@@ -1733,7 +1737,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>28</v>
@@ -1805,7 +1809,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
correct DOM load sequencing for saved queries
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -874,7 +874,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1326,26 +1326,30 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="A18" s="12">
         <v>37</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="C18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="F18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="13">
+        <v>43033</v>
+      </c>
+      <c r="H18" s="13">
+        <v>43033</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">

</xml_diff>

<commit_message>
added basic table sorting on value
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$44</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="97">
   <si>
     <t>Feature</t>
   </si>
@@ -287,6 +287,39 @@
   </si>
   <si>
     <t>Like excel pivot tables. Rendering controlled by a flag, which we can add to the UI at a later point.</t>
+  </si>
+  <si>
+    <t>Sort pivot table by values, asc/desc</t>
+  </si>
+  <si>
+    <t>Add x-axis tick mark labels to chart</t>
+  </si>
+  <si>
+    <t>Look in docs for how to do this</t>
+  </si>
+  <si>
+    <t>Change chart value tooltips to read "Foo" instead of "count(CASENUMBER) of Foo: $Value"</t>
+  </si>
+  <si>
+    <t>Chart labels should reflect row/col labels from pivot table</t>
+  </si>
+  <si>
+    <t>I think we're reading these labels from Model, not the transform.</t>
+  </si>
+  <si>
+    <t>Add views, in addition to tables, to data sources</t>
+  </si>
+  <si>
+    <t>Possible bug: are charts reflecting/working with filters are selected?</t>
+  </si>
+  <si>
+    <t>Do some more testing with large numbers of selected filter values. That might be the issue.</t>
+  </si>
+  <si>
+    <t>When sort-by-value is indicated (on an aggregator column cell), save row coord + agg coord + (asc | desc) in a the transformation. If sort-by-value transformation key is found, create a sequence of {row-coord: Array, value: (Number | String)} and then: natural sort the sequence on value key -&gt; return a sequence of just the row coord keys. Then render the pivot table using this new row coord ordering rather than the one returned by the cartesian coords fn.</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -317,12 +350,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -337,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -389,6 +428,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,10 +904,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -953,7 +1001,7 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>26</v>
       </c>
@@ -1184,7 +1232,7 @@
         <v>42965</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>17</v>
       </c>
@@ -1262,7 +1310,7 @@
         <v>43004</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>32</v>
       </c>
@@ -1314,7 +1362,7 @@
         <v>43019</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>37</v>
       </c>
@@ -1366,23 +1414,23 @@
         <v>43006</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="3" t="s">
+    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <v>41</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1542,49 +1590,49 @@
         <v>42999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>21</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="3" t="s">
+    <row r="27" spans="1:8" s="15" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>38</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="16">
+        <v>43045</v>
+      </c>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <v>39</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
-        <v>19</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
     </row>
     <row r="29" spans="1:8" ht="51" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
@@ -1768,23 +1816,23 @@
         <v>42984</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>22</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F36" s="3" t="s">
+    <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="18">
+        <v>40</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" s="18" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1814,35 +1862,161 @@
         <v>42999</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>9</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="11" t="s">
+    <row r="38" spans="1:8" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <v>43</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
+    <row r="39" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>21</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>19</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="16">
+        <v>43035</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>9</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H38">
+  <autoFilter ref="A1:H44">
     <filterColumn colId="5">
       <filters>
         <filter val="Not Started"/>
       </filters>
     </filterColumn>
+    <sortState ref="A20:H44">
+      <sortCondition ref="C2:C44" customList="HIGH,MED,LOW"/>
+      <sortCondition ref="D2:D44" customList="LOW,MED,HIGH"/>
+    </sortState>
   </autoFilter>
   <sortState ref="A2:H38">
     <sortCondition ref="C2:C38" customList="HIGH,MED,LOW"/>

</xml_diff>

<commit_message>
center chart title and editable chart title
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$50</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="107">
   <si>
     <t>Feature</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Bug: identical Value entries cause 'column ambiguously defined' (e.g. COUNTOF_ID and COUNTOF_ID in Values bucket)</t>
   </si>
   <si>
-    <t>Logging user behavior data. Foreign key of query, and whether a chart was used (and which chart)</t>
-  </si>
-  <si>
     <t>Display chart representation of pivot table with chart.js. Simple bar/line charts for now.</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Will write a logging library that can be called with arbitrary JS objects to store information. How to generate &amp; track user IDs?</t>
-  </si>
-  <si>
     <t>Some data contortion required. Array of arrays not supported in the case of multiple aggregators. Also, what about case of non-numeric fields? (Labels will be improved with #11)</t>
   </si>
   <si>
@@ -295,9 +289,6 @@
     <t>Add x-axis tick mark labels to chart</t>
   </si>
   <si>
-    <t>Look in docs for how to do this</t>
-  </si>
-  <si>
     <t>Change chart value tooltips to read "Foo" instead of "count(CASENUMBER) of Foo: $Value"</t>
   </si>
   <si>
@@ -319,13 +310,46 @@
     <t>Can't remove value (e.g. the number for this row/col intersection)</t>
   </si>
   <si>
-    <t>This seems to be working? May be wonky with large filter sets applied.</t>
-  </si>
-  <si>
     <t>Charts should work when there are no aggregators</t>
   </si>
   <si>
     <t>Charts were incorrectly referencing model.Values to get agg list, causing NPEs. Switched to results.meta.aggregators and it's working.</t>
+  </si>
+  <si>
+    <t>Added tick marks and improved legibility (with line breaks). Also fixed an issue where bars, tick marks, and tick mark text were misaligned.</t>
+  </si>
+  <si>
+    <t>This seems to be working? May be wonky with large filter sets applied. Will continute to monitor.</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>change field-level manipulations on pivot table to dropdown-based, like in Excel.</t>
+  </si>
+  <si>
+    <t>Thereby removing the mouseover buttons we currently use</t>
+  </si>
+  <si>
+    <t>charts should intelligently flip x/y axes so that primary axis is always X. Like in Excel.</t>
+  </si>
+  <si>
+    <t>Logging user behavior data. Save each request made to server: model data + transform + action type ( load | request | chart)</t>
+  </si>
+  <si>
+    <t>Also include columns created_date updated_date expire_date user</t>
+  </si>
+  <si>
+    <t>Chart title should be centered.</t>
+  </si>
+  <si>
+    <t>Chart title should be editable. Save in transform.</t>
+  </si>
+  <si>
+    <t>Should be able to sort pivot table labels.</t>
+  </si>
+  <si>
+    <t>Part of #48</t>
   </si>
 </sst>
 </file>
@@ -382,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -395,15 +419,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -444,8 +459,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,10 +934,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -929,36 +950,36 @@
     <col min="6" max="6" width="11.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="14"/>
+    <col min="9" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" s="10" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>6</v>
       </c>
@@ -977,10 +998,10 @@
       <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="13">
         <v>42972</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="13">
         <v>42972</v>
       </c>
     </row>
@@ -1003,62 +1024,62 @@
       <c r="F3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="13">
         <v>42972</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="13">
         <v>42972</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="8">
         <v>26</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="12">
+      <c r="B4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="9">
         <v>43031</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="9">
         <v>43031</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+    <row r="5" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="12">
+      <c r="B5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="9">
         <v>43006</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="9">
         <v>43006</v>
       </c>
     </row>
@@ -1067,7 +1088,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1078,10 +1099,10 @@
       <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="13">
         <v>43020</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="13">
         <v>43020</v>
       </c>
     </row>
@@ -1090,7 +1111,7 @@
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1099,15 +1120,15 @@
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="13">
         <v>43019</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="13">
         <v>43020</v>
       </c>
     </row>
@@ -1116,7 +1137,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1125,15 +1146,15 @@
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="13">
         <v>43003</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="13">
         <v>43003</v>
       </c>
     </row>
@@ -1142,7 +1163,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -1151,15 +1172,15 @@
         <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="13">
         <v>42965</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="13">
         <v>42974</v>
       </c>
     </row>
@@ -1182,10 +1203,10 @@
       <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="13">
         <v>42975</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="13">
         <v>42975</v>
       </c>
     </row>
@@ -1194,7 +1215,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -1203,19 +1224,19 @@
         <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="13">
         <v>42976</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <v>42977</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="15" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="12" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>7</v>
       </c>
@@ -1242,28 +1263,28 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="8">
         <v>17</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="9">
         <v>43032</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="9">
         <v>43032</v>
       </c>
     </row>
@@ -1272,76 +1293,76 @@
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="9">
+        <v>43004</v>
+      </c>
+      <c r="H14" s="9">
+        <v>43005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="12" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="12">
+      <c r="F15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="9">
         <v>43004</v>
       </c>
-      <c r="H14" s="12">
-        <v>43005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="15" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>31</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="H15" s="9">
+        <v>43004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>32</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="12">
-        <v>43004</v>
-      </c>
-      <c r="H15" s="12">
-        <v>43004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>32</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="9">
         <v>43034</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="9">
         <v>43034</v>
       </c>
     </row>
@@ -1350,7 +1371,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1359,41 +1380,41 @@
         <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="13">
         <v>43018</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="13">
         <v>43019</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="8">
         <v>37</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="12">
+      <c r="B18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="9">
         <v>43033</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="9">
         <v>43033</v>
       </c>
     </row>
@@ -1401,51 +1422,51 @@
       <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="12">
+      <c r="C19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="9">
         <v>43006</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="9">
         <v>43006</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
+    <row r="20" spans="1:8" s="12" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
         <v>41</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="16">
+      <c r="B20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="9">
         <v>43049</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="9">
         <v>43049</v>
       </c>
     </row>
@@ -1453,7 +1474,7 @@
       <c r="A21" s="3">
         <v>11</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1462,16 +1483,16 @@
       <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>62</v>
+      <c r="E21" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="13">
         <v>42976</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="9">
         <v>42992</v>
       </c>
     </row>
@@ -1489,15 +1510,15 @@
         <v>4</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="13">
         <v>42978</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="13">
         <v>42978</v>
       </c>
     </row>
@@ -1541,15 +1562,15 @@
         <v>6</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="13">
         <v>42996</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="13">
         <v>42996</v>
       </c>
     </row>
@@ -1572,10 +1593,10 @@
       <c r="F25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="13">
         <v>42984</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="13">
         <v>42984</v>
       </c>
     </row>
@@ -1584,7 +1605,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -1593,67 +1614,67 @@
         <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="13">
         <v>42999</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="13">
         <v>42999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="15" customFormat="1" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
+    <row r="27" spans="1:8" s="12" customFormat="1" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
         <v>38</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="16">
+      <c r="B27" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="13">
         <v>43045</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="13">
         <v>43048</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="18">
+    <row r="28" spans="1:8" s="12" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
         <v>39</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="16">
+      <c r="B28" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="9">
         <v>43049</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="9">
         <v>43049</v>
       </c>
     </row>
@@ -1676,10 +1697,10 @@
       <c r="F29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="16">
+      <c r="G29" s="13">
         <v>42964</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="13">
         <v>42976</v>
       </c>
     </row>
@@ -1688,7 +1709,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
@@ -1697,15 +1718,15 @@
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="13">
         <v>42996</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="13">
         <v>42996</v>
       </c>
     </row>
@@ -1713,25 +1734,25 @@
       <c r="A31" s="3">
         <v>15</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="12">
+      <c r="B31" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="9">
         <v>43005</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="9">
         <v>43006</v>
       </c>
     </row>
@@ -1761,29 +1782,29 @@
         <v>42965</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="15" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="12" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F33" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="16">
+      <c r="G33" s="13">
         <v>42979</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H33" s="13">
         <v>42979</v>
       </c>
     </row>
@@ -1792,7 +1813,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
@@ -1801,15 +1822,15 @@
         <v>4</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="13">
         <v>43003</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34" s="13">
         <v>43003</v>
       </c>
     </row>
@@ -1818,7 +1839,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>4</v>
@@ -1827,41 +1848,41 @@
         <v>6</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="16">
+      <c r="G35" s="13">
         <v>42979</v>
       </c>
-      <c r="H35" s="16">
+      <c r="H35" s="13">
         <v>42984</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18">
+    <row r="36" spans="1:8" s="12" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
         <v>40</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="16">
+      <c r="B36" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="9">
         <v>43049</v>
       </c>
-      <c r="H36" s="16">
+      <c r="H36" s="9">
         <v>43049</v>
       </c>
     </row>
@@ -1879,50 +1900,50 @@
         <v>5</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="9">
         <v>42990</v>
       </c>
-      <c r="H37" s="12">
+      <c r="H37" s="9">
         <v>42999</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="18">
+    <row r="38" spans="1:8" s="12" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
         <v>43</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="19" t="s">
+      <c r="B38" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F38" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" s="16">
+      <c r="F38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="9">
         <v>43049</v>
       </c>
-      <c r="H38" s="16">
+      <c r="H38" s="9">
         <v>43049</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="51" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>6</v>
@@ -1931,35 +1952,43 @@
         <v>6</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
-        <v>19</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-    </row>
-    <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G39" s="9">
+        <v>43049</v>
+      </c>
+      <c r="H39" s="9">
+        <v>43049</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>47</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="16"/>
+      <c r="F40" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="9">
+        <v>43059</v>
+      </c>
+      <c r="H40" s="9">
+        <v>43059</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="51" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>1</v>
       </c>
@@ -1976,35 +2005,37 @@
         <v>24</v>
       </c>
       <c r="F41" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>45</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F42" s="15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>22</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
@@ -2015,66 +2046,178 @@
       <c r="F43" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="16">
+      <c r="G43" s="13">
         <v>43035</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+    <row r="44" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>46</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="16"/>
+      <c r="F44" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="9">
+        <v>43059</v>
+      </c>
+      <c r="H44" s="9">
+        <v>43059</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="12" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="9">
+        <v>43049</v>
+      </c>
+      <c r="H45" s="9">
+        <v>43049</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>48</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>49</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="16"/>
+      <c r="F47" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
+        <v>19</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>22</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
         <v>9</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B50" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="9" t="s">
+      <c r="C50" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F50" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="18">
-        <v>44</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G45" s="21">
-        <v>43049</v>
-      </c>
-      <c r="H45" s="21">
-        <v>43049</v>
-      </c>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H44">
+  <autoFilter ref="A1:H50">
     <filterColumn colId="5">
       <filters>
         <filter val="Not Started"/>
       </filters>
     </filterColumn>
-    <sortState ref="A20:H44">
-      <sortCondition ref="C2:C44" customList="HIGH,MED,LOW"/>
-      <sortCondition ref="D2:D44" customList="LOW,MED,HIGH"/>
+    <sortState ref="A40:H50">
+      <sortCondition ref="C2:C50" customList="HIGH,MED,LOW"/>
+      <sortCondition ref="D2:D50" customList="LOW,MED,HIGH"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:H38">

</xml_diff>

<commit_message>
server-side save/load for queries
</commit_message>
<xml_diff>
--- a/tracking/tpivot-phase-3-tracking.xlsx
+++ b/tracking/tpivot-phase-3-tracking.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$51</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="109">
   <si>
     <t>Feature</t>
   </si>
@@ -334,12 +334,6 @@
     <t>charts should intelligently flip x/y axes so that primary axis is always X. Like in Excel.</t>
   </si>
   <si>
-    <t>Logging user behavior data. Save each request made to server: model data + transform + action type ( load | request | chart)</t>
-  </si>
-  <si>
-    <t>Also include columns created_date updated_date expire_date user</t>
-  </si>
-  <si>
     <t>Chart title should be centered.</t>
   </si>
   <si>
@@ -350,6 +344,18 @@
   </si>
   <si>
     <t>Part of #48</t>
+  </si>
+  <si>
+    <t>User can define 'save name' for query</t>
+  </si>
+  <si>
+    <t>ID, QUERY_NAME, USER, MODEL, TRANSFORM, EVENT, CREATE_DATE, UPDATE_DATE, UPDATE_USER, EXPIRE_DATE, EXPIRE_USER</t>
+  </si>
+  <si>
+    <t>Save queries to server.</t>
+  </si>
+  <si>
+    <t>part of #19</t>
   </si>
 </sst>
 </file>
@@ -934,10 +940,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1964,21 +1970,21 @@
         <v>43049</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>47</v>
       </c>
-      <c r="B40" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="16"/>
-      <c r="F40" s="15" t="s">
+      <c r="B40" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G40" s="9">
@@ -2008,23 +2014,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
-        <v>45</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="F42" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="8" t="s">
         <v>25</v>
       </c>
       <c r="G42" s="8"/>
@@ -2050,21 +2054,21 @@
         <v>43035</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>46</v>
       </c>
-      <c r="B44" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="15" t="s">
+      <c r="B44" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="6"/>
+      <c r="F44" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G44" s="9">
@@ -2100,85 +2104,95 @@
         <v>43049</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
-        <v>48</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="13">
+        <v>43061</v>
+      </c>
+      <c r="H46" s="13">
+        <v>43061</v>
+      </c>
     </row>
     <row r="47" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
-        <v>49</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47" s="16"/>
-      <c r="F47" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-    </row>
-    <row r="48" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" s="9">
+        <v>43062</v>
+      </c>
+      <c r="H47" s="9">
+        <v>43062</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
-        <v>19</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F48" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F48" s="8" t="s">
         <v>25</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="8">
-        <v>22</v>
+    <row r="49" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
+        <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>25</v>
@@ -2188,19 +2202,19 @@
     </row>
     <row r="50" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>25</v>
@@ -2208,16 +2222,38 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
     </row>
+    <row r="51" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>9</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H50">
+  <autoFilter ref="A1:H51">
     <filterColumn colId="5">
       <filters>
         <filter val="Not Started"/>
       </filters>
     </filterColumn>
-    <sortState ref="A40:H50">
-      <sortCondition ref="C2:C50" customList="HIGH,MED,LOW"/>
-      <sortCondition ref="D2:D50" customList="LOW,MED,HIGH"/>
+    <sortState ref="A42:H51">
+      <sortCondition ref="C2:C51" customList="HIGH,MED,LOW"/>
+      <sortCondition ref="D2:D51" customList="LOW,MED,HIGH"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:H38">

</xml_diff>